<commit_message>
added opiod conversion factors as global variables
</commit_message>
<xml_diff>
--- a/mme_conversion/MME Conversion Factors.xlsx
+++ b/mme_conversion/MME Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackallan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackallan/Dropbox/KGrid/CPIC-objects/mme_conversion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4546D5F4-FB66-DB4A-9022-C2954952EEB4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168A73D5-CADA-A141-8EBF-058A84A45373}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{5F6B5230-3932-3F45-99B5-7D1BA5662790}"/>
+    <workbookView xWindow="2800" yWindow="1540" windowWidth="28040" windowHeight="17440" xr2:uid="{5F6B5230-3932-3F45-99B5-7D1BA5662790}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">CALCULATING TOTAL DAILY DOSE 
 </t>
@@ -98,7 +97,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">OF OPIOIDS FOR SAFER DOSAGE"
 </t>
@@ -109,7 +107,6 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -120,14 +117,13 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve"> 
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{23D1D246-B169-DC4E-B1BD-52225C38B949}">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{23D1D246-B169-DC4E-B1BD-52225C38B949}">
       <text>
         <r>
           <rPr>
@@ -331,7 +327,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -674,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF00A21A-C8EF-7E42-88AF-C98DA8FE66B4}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,58 +787,69 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>30</v>
+      </c>
+    </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>30</v>
+        <v>12.6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15">
-        <v>12.6</v>
+        <v>0.03</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B16">
-        <v>0.03</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18">
-        <v>0.25</v>
+        <v>0.13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -851,10 +857,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
@@ -862,10 +868,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>0.16</v>
+        <v>7.2</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -873,60 +879,49 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B22">
-        <v>7.2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26">
-        <v>0.37</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>